<commit_message>
case studies discussion and figures
</commit_message>
<xml_diff>
--- a/results/results_mutualSeparation.xlsx
+++ b/results/results_mutualSeparation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Documents\Repositories\distributed-monitoring\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EC8DAC-D9D4-437F-AC55-6A95971B1F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE6B756-4CE5-40EA-ACF6-20BC0B076939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="4245" windowWidth="21600" windowHeight="12765" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
   <si>
     <t>d = 0.5 seconds (10 samples at 20Hz)</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>SMT/F-RELATIVE</t>
+  </si>
+  <si>
+    <t>SMT/FINE</t>
   </si>
 </sst>
 </file>
@@ -311,8 +314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,66 +790,131 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <f>B9/B6</f>
+        <f t="shared" ref="B14:G14" si="1">B9/B6</f>
         <v>3835.3675257347732</v>
       </c>
       <c r="C14" s="2">
-        <f>C9/C6</f>
+        <f t="shared" si="1"/>
         <v>1594.7492196165804</v>
       </c>
       <c r="D14" s="2">
-        <f>D9/D6</f>
+        <f t="shared" si="1"/>
         <v>1372.7629512753972</v>
       </c>
       <c r="E14" s="2">
-        <f>E9/E6</f>
+        <f t="shared" si="1"/>
         <v>711.51739146324883</v>
       </c>
       <c r="F14" s="2">
-        <f>F9/F6</f>
+        <f t="shared" si="1"/>
         <v>270.85333798142688</v>
       </c>
       <c r="G14" s="2">
-        <f>G9/G6</f>
+        <f t="shared" si="1"/>
         <v>24249.86242919456</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" ref="H14:P14" si="1">H9/H6</f>
+        <f t="shared" ref="H14:P14" si="2">H9/H6</f>
         <v>12996.913066835143</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8778.8809139727709</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2509.0311250597779</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1017.2024020001307</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78420.863456410923</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59032.051917631317</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25854.847765907063</v>
       </c>
       <c r="O14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9653.2175581841002</v>
       </c>
       <c r="P14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4912.0866907173067</v>
       </c>
       <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <f>B9/B5</f>
+        <v>653.9718725613991</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:P15" si="3">C9/C5</f>
+        <v>256.49833021329482</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="3"/>
+        <v>26.523465847542269</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>1.8809050306220272</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>0.17334817016506315</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>4863.4744895436934</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>749.78939691448284</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>115.72922456832265</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>6.7170490496508481</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>0.64190021790673479</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>16383.262808219453</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>3412.6800978997921</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>337.45793981645289</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>26.019929855695032</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>3.2164365740020706</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>